<commit_message>
Create second test case for calculateMass function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AF5A591-4C8D-4994-BDF2-365F2D1A810A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F001B8CE-9B61-45A9-BA42-DBA51E74F474}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Test case 1</t>
+  </si>
+  <si>
+    <t>Test case 2</t>
+  </si>
+  <si>
+    <t>UT_002</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,28 +199,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -225,6 +219,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,47 +565,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2">
@@ -604,22 +613,22 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -627,34 +636,140 @@
       <c r="A8" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="7">
         <v>3</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="7">
         <v>3</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4">
+      <c r="B9" s="7"/>
+      <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="12"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>1</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
Create third test case for calculateMass function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F001B8CE-9B61-45A9-BA42-DBA51E74F474}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEBEE37-8268-4BA1-8F8C-7F36D2233362}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>UT_002</t>
+  </si>
+  <si>
+    <t>Test case 3</t>
   </si>
 </sst>
 </file>
@@ -188,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -220,19 +223,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,10 +590,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -595,8 +604,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -633,34 +642,34 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="15">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="16">
         <v>3</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="16">
         <v>3</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
@@ -679,10 +688,10 @@
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -693,8 +702,8 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="15"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -731,37 +740,151 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="15">
         <v>1</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="16">
         <v>2</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="16">
         <v>2</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>1</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8</v>
+      </c>
+      <c r="D28" s="16">
+        <v>2</v>
+      </c>
+      <c r="E28" s="16">
+        <v>2</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="7">
+        <v>4</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="24">
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
@@ -770,14 +893,6 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Create test case for calculateAcceleration function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEBEE37-8268-4BA1-8F8C-7F36D2233362}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB9BBEC-1880-4689-8526-F7A558AE59E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Test case 3</t>
+  </si>
+  <si>
+    <t>Test case 4</t>
+  </si>
+  <si>
+    <t>Test the function: calculateAcceleration</t>
+  </si>
+  <si>
+    <t>Testing calculateAcceleration function</t>
   </si>
 </sst>
 </file>
@@ -191,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,6 +224,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -558,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,14 +589,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -590,10 +605,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -604,8 +619,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -642,44 +657,44 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="17">
         <v>1</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="18">
         <v>3</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="18">
         <v>3</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -688,10 +703,10 @@
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -702,8 +717,8 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -740,44 +755,44 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="A18" s="17">
         <v>1</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="18">
         <v>2</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="18">
         <v>2</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -786,10 +801,10 @@
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -800,8 +815,8 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -838,37 +853,159 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="17">
         <v>1</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1">
         <v>8</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="18">
         <v>2</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="18">
         <v>2</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="16"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <v>1</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="1">
+        <v>8</v>
+      </c>
+      <c r="D38" s="18">
+        <v>4</v>
+      </c>
+      <c r="E38" s="18">
+        <v>4</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="10">
+        <v>2</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="32">
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
@@ -877,22 +1014,6 @@
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Create second test case for calculateAcceleration function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB9BBEC-1880-4689-8526-F7A558AE59E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D668E6BC-35EC-438B-BFF1-4D13EFF8C162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Testing calculateAcceleration function</t>
+  </si>
+  <si>
+    <t>Test case 5</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +227,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -573,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,14 +598,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -605,10 +614,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -619,8 +628,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -657,44 +666,44 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="19">
         <v>1</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="20">
         <v>3</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="20">
         <v>3</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -703,10 +712,10 @@
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -717,8 +726,8 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -755,44 +764,44 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="19">
         <v>1</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="18">
-        <v>2</v>
-      </c>
-      <c r="E18" s="18">
-        <v>2</v>
-      </c>
-      <c r="F18" s="19" t="s">
+      <c r="D18" s="20">
+        <v>2</v>
+      </c>
+      <c r="E18" s="20">
+        <v>2</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -801,10 +810,10 @@
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="15" t="s">
+      <c r="C23" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -815,8 +824,8 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -853,44 +862,44 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+      <c r="A28" s="19">
         <v>1</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1">
         <v>8</v>
       </c>
-      <c r="D28" s="18">
-        <v>2</v>
-      </c>
-      <c r="E28" s="18">
-        <v>2</v>
-      </c>
-      <c r="F28" s="19" t="s">
+      <c r="D28" s="20">
+        <v>2</v>
+      </c>
+      <c r="E28" s="20">
+        <v>2</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
     </row>
     <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -899,10 +908,10 @@
       <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="15" t="s">
+      <c r="C33" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -913,8 +922,8 @@
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -951,37 +960,167 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+      <c r="A38" s="19">
         <v>1</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="1">
         <v>8</v>
       </c>
-      <c r="D38" s="18">
-        <v>4</v>
-      </c>
-      <c r="E38" s="18">
-        <v>4</v>
-      </c>
-      <c r="F38" s="19" t="s">
+      <c r="D38" s="20">
+        <v>4</v>
+      </c>
+      <c r="E38" s="20">
+        <v>4</v>
+      </c>
+      <c r="F38" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="18"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="10">
         <v>2</v>
       </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+    </row>
+    <row r="41" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A41" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="18"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="19">
+        <v>1</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="1">
+        <v>16</v>
+      </c>
+      <c r="D48" s="20">
+        <v>2</v>
+      </c>
+      <c r="E48" s="20">
+        <v>2</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="12">
+        <v>4</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="40">
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="D33:D34"/>
@@ -990,30 +1129,6 @@
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="F38:F39"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Create third test case for calculateAcceleration function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D668E6BC-35EC-438B-BFF1-4D13EFF8C162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54EDFF0-327F-4ABD-ACD6-0FD024E6B53E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Test case 5</t>
+  </si>
+  <si>
+    <t>Test case 6</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +230,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -582,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,14 +607,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -614,10 +623,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -628,8 +637,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -666,44 +675,44 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="21">
         <v>1</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="22">
         <v>3</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="22">
         <v>3</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -712,10 +721,10 @@
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -726,8 +735,8 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -764,44 +773,44 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="21">
         <v>1</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="20">
-        <v>2</v>
-      </c>
-      <c r="E18" s="20">
-        <v>2</v>
-      </c>
-      <c r="F18" s="21" t="s">
+      <c r="D18" s="22">
+        <v>2</v>
+      </c>
+      <c r="E18" s="22">
+        <v>2</v>
+      </c>
+      <c r="F18" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -810,10 +819,10 @@
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="17" t="s">
+      <c r="C23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -824,8 +833,8 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="20"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -862,44 +871,44 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="21">
         <v>1</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1">
         <v>8</v>
       </c>
-      <c r="D28" s="20">
-        <v>2</v>
-      </c>
-      <c r="E28" s="20">
-        <v>2</v>
-      </c>
-      <c r="F28" s="21" t="s">
+      <c r="D28" s="22">
+        <v>2</v>
+      </c>
+      <c r="E28" s="22">
+        <v>2</v>
+      </c>
+      <c r="F28" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -908,10 +917,10 @@
       <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="17" t="s">
+      <c r="C33" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -922,8 +931,8 @@
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="20"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -960,44 +969,44 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
+      <c r="A38" s="21">
         <v>1</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="1">
         <v>8</v>
       </c>
-      <c r="D38" s="20">
-        <v>4</v>
-      </c>
-      <c r="E38" s="20">
-        <v>4</v>
-      </c>
-      <c r="F38" s="21" t="s">
+      <c r="D38" s="22">
+        <v>4</v>
+      </c>
+      <c r="E38" s="22">
+        <v>4</v>
+      </c>
+      <c r="F38" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="10">
         <v>2</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="23"/>
     </row>
     <row r="41" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -1006,10 +1015,10 @@
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="17" t="s">
+      <c r="C43" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1020,8 +1029,8 @@
       <c r="B44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="20"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -1058,37 +1067,175 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
+      <c r="A48" s="21">
         <v>1</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="1">
         <v>16</v>
       </c>
-      <c r="D48" s="20">
-        <v>2</v>
-      </c>
-      <c r="E48" s="20">
-        <v>2</v>
-      </c>
-      <c r="F48" s="21" t="s">
+      <c r="D48" s="22">
+        <v>2</v>
+      </c>
+      <c r="E48" s="22">
+        <v>2</v>
+      </c>
+      <c r="F48" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="12">
         <v>4</v>
       </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="21"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="23"/>
+    </row>
+    <row r="51" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A51" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="20"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
+        <v>1</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="1">
+        <v>9</v>
+      </c>
+      <c r="D58" s="22">
+        <v>2</v>
+      </c>
+      <c r="E58" s="22">
+        <v>2</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="14">
+        <v>3</v>
+      </c>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="48">
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
     <mergeCell ref="A41:F41"/>
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="D43:D44"/>
@@ -1097,38 +1244,6 @@
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="F48:F49"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Create test case for calculateVolume function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54EDFF0-327F-4ABD-ACD6-0FD024E6B53E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17121364-D718-4A4E-9976-89606400D411}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>Test case 6</t>
+  </si>
+  <si>
+    <t>Test case 7</t>
+  </si>
+  <si>
+    <t>Test the function: calculateVolume</t>
+  </si>
+  <si>
+    <t>Testing calculateVolume function</t>
   </si>
 </sst>
 </file>
@@ -206,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,6 +239,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -591,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,14 +622,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -623,10 +638,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -637,8 +652,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -675,44 +690,44 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="23">
         <v>1</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="24">
         <v>3</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="24">
         <v>3</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -721,10 +736,10 @@
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -735,8 +750,8 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="22"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -773,44 +788,44 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="23">
         <v>1</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="22">
-        <v>2</v>
-      </c>
-      <c r="E18" s="22">
-        <v>2</v>
-      </c>
-      <c r="F18" s="23" t="s">
+      <c r="D18" s="24">
+        <v>2</v>
+      </c>
+      <c r="E18" s="24">
+        <v>2</v>
+      </c>
+      <c r="F18" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -819,10 +834,10 @@
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="19" t="s">
+      <c r="C23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -833,8 +848,8 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -871,44 +886,44 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
+      <c r="A28" s="23">
         <v>1</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1">
         <v>8</v>
       </c>
-      <c r="D28" s="22">
-        <v>2</v>
-      </c>
-      <c r="E28" s="22">
-        <v>2</v>
-      </c>
-      <c r="F28" s="23" t="s">
+      <c r="D28" s="24">
+        <v>2</v>
+      </c>
+      <c r="E28" s="24">
+        <v>2</v>
+      </c>
+      <c r="F28" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -917,10 +932,10 @@
       <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="19" t="s">
+      <c r="C33" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -931,8 +946,8 @@
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="22"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -969,44 +984,44 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="21">
+      <c r="A38" s="23">
         <v>1</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="1">
         <v>8</v>
       </c>
-      <c r="D38" s="22">
-        <v>4</v>
-      </c>
-      <c r="E38" s="22">
-        <v>4</v>
-      </c>
-      <c r="F38" s="23" t="s">
+      <c r="D38" s="24">
+        <v>4</v>
+      </c>
+      <c r="E38" s="24">
+        <v>4</v>
+      </c>
+      <c r="F38" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="10">
         <v>2</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="23"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
     </row>
     <row r="41" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -1015,10 +1030,10 @@
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="19" t="s">
+      <c r="C43" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1029,8 +1044,8 @@
       <c r="B44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="22"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -1067,44 +1082,44 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="21">
+      <c r="A48" s="23">
         <v>1</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="1">
         <v>16</v>
       </c>
-      <c r="D48" s="22">
-        <v>2</v>
-      </c>
-      <c r="E48" s="22">
-        <v>2</v>
-      </c>
-      <c r="F48" s="23" t="s">
+      <c r="D48" s="24">
+        <v>2</v>
+      </c>
+      <c r="E48" s="24">
+        <v>2</v>
+      </c>
+      <c r="F48" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
-      <c r="B49" s="22"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="12">
         <v>4</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="25"/>
     </row>
     <row r="51" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
@@ -1113,10 +1128,10 @@
       <c r="B53" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" s="19" t="s">
+      <c r="C53" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1127,8 +1142,8 @@
       <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="22"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -1165,37 +1180,183 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="21">
+      <c r="A58" s="23">
         <v>1</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C58" s="1">
         <v>9</v>
       </c>
-      <c r="D58" s="22">
-        <v>2</v>
-      </c>
-      <c r="E58" s="22">
-        <v>2</v>
-      </c>
-      <c r="F58" s="23" t="s">
+      <c r="D58" s="24">
+        <v>2</v>
+      </c>
+      <c r="E58" s="24">
+        <v>2</v>
+      </c>
+      <c r="F58" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="14">
         <v>3</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="23"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="25"/>
+    </row>
+    <row r="61" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A61" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="20"/>
+      <c r="D64" s="22"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="23">
+        <v>1</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="1">
+        <v>20</v>
+      </c>
+      <c r="D68" s="24">
+        <v>3768</v>
+      </c>
+      <c r="E68" s="24">
+        <v>3768</v>
+      </c>
+      <c r="F68" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="23"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="16">
+        <v>3</v>
+      </c>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="56">
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
     <mergeCell ref="A51:F51"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
@@ -1204,46 +1365,6 @@
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="E58:E59"/>
     <mergeCell ref="F58:F59"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Create second test case for calculateVolume function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17121364-D718-4A4E-9976-89606400D411}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EA1DB1-9AC5-411B-AE53-922A8A431F0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Testing calculateVolume function</t>
+  </si>
+  <si>
+    <t>Test case 8</t>
   </si>
 </sst>
 </file>
@@ -215,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +242,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,14 +631,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -638,10 +647,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -652,8 +661,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -690,44 +699,44 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="25">
         <v>1</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="26">
         <v>3</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="26">
         <v>3</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -736,10 +745,10 @@
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -750,8 +759,8 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -788,44 +797,44 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
+      <c r="A18" s="25">
         <v>1</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="24">
-        <v>2</v>
-      </c>
-      <c r="E18" s="24">
-        <v>2</v>
-      </c>
-      <c r="F18" s="25" t="s">
+      <c r="D18" s="26">
+        <v>2</v>
+      </c>
+      <c r="E18" s="26">
+        <v>2</v>
+      </c>
+      <c r="F18" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -834,10 +843,10 @@
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="21" t="s">
+      <c r="C23" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -848,8 +857,8 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="24"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -886,44 +895,44 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="25">
         <v>1</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1">
         <v>8</v>
       </c>
-      <c r="D28" s="24">
-        <v>2</v>
-      </c>
-      <c r="E28" s="24">
-        <v>2</v>
-      </c>
-      <c r="F28" s="25" t="s">
+      <c r="D28" s="26">
+        <v>2</v>
+      </c>
+      <c r="E28" s="26">
+        <v>2</v>
+      </c>
+      <c r="F28" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="25"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
     </row>
     <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -932,10 +941,10 @@
       <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="21" t="s">
+      <c r="C33" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -946,8 +955,8 @@
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="24"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -984,44 +993,44 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="23">
+      <c r="A38" s="25">
         <v>1</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="1">
         <v>8</v>
       </c>
-      <c r="D38" s="24">
-        <v>4</v>
-      </c>
-      <c r="E38" s="24">
-        <v>4</v>
-      </c>
-      <c r="F38" s="25" t="s">
+      <c r="D38" s="26">
+        <v>4</v>
+      </c>
+      <c r="E38" s="26">
+        <v>4</v>
+      </c>
+      <c r="F38" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="10">
         <v>2</v>
       </c>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="25"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="27"/>
     </row>
     <row r="41" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -1030,10 +1039,10 @@
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="21" t="s">
+      <c r="C43" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1044,8 +1053,8 @@
       <c r="B44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="24"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -1082,44 +1091,44 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="23">
+      <c r="A48" s="25">
         <v>1</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="1">
         <v>16</v>
       </c>
-      <c r="D48" s="24">
-        <v>2</v>
-      </c>
-      <c r="E48" s="24">
-        <v>2</v>
-      </c>
-      <c r="F48" s="25" t="s">
+      <c r="D48" s="26">
+        <v>2</v>
+      </c>
+      <c r="E48" s="26">
+        <v>2</v>
+      </c>
+      <c r="F48" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="12">
         <v>4</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="25"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="27"/>
     </row>
     <row r="51" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
@@ -1128,10 +1137,10 @@
       <c r="B53" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" s="21" t="s">
+      <c r="C53" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1142,8 +1151,8 @@
       <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -1180,44 +1189,44 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="23">
+      <c r="A58" s="25">
         <v>1</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C58" s="1">
         <v>9</v>
       </c>
-      <c r="D58" s="24">
-        <v>2</v>
-      </c>
-      <c r="E58" s="24">
-        <v>2</v>
-      </c>
-      <c r="F58" s="25" t="s">
+      <c r="D58" s="26">
+        <v>2</v>
+      </c>
+      <c r="E58" s="26">
+        <v>2</v>
+      </c>
+      <c r="F58" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="24"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="14">
         <v>3</v>
       </c>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="25"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="27"/>
     </row>
     <row r="61" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
@@ -1226,10 +1235,10 @@
       <c r="B63" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D63" s="21" t="s">
+      <c r="C63" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1240,8 +1249,8 @@
       <c r="B64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="20"/>
-      <c r="D64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="24"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
@@ -1278,37 +1287,191 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
+      <c r="A68" s="25">
         <v>1</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C68" s="1">
         <v>20</v>
       </c>
-      <c r="D68" s="24">
+      <c r="D68" s="26">
         <v>3768</v>
       </c>
-      <c r="E68" s="24">
+      <c r="E68" s="26">
         <v>3768</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F68" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
-      <c r="B69" s="24"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="16">
         <v>3</v>
       </c>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="25"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="27"/>
+    </row>
+    <row r="71" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A71" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="22"/>
+      <c r="D74" s="24"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="25">
+        <v>1</v>
+      </c>
+      <c r="B78" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" s="1">
+        <v>5</v>
+      </c>
+      <c r="D78" s="26">
+        <v>157</v>
+      </c>
+      <c r="E78" s="26">
+        <v>157</v>
+      </c>
+      <c r="F78" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="25"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="18">
+        <v>2</v>
+      </c>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="64">
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="C63:C64"/>
     <mergeCell ref="D63:D64"/>
@@ -1317,54 +1480,6 @@
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
     <mergeCell ref="F68:F69"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Create third test case for calculateVolume function
</commit_message>
<xml_diff>
--- a/Documentation and Prezentation/QA.xlsx
+++ b/Documentation and Prezentation/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Documents\GitHub\PhysicsProject-2021\Documentation and Prezentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EA1DB1-9AC5-411B-AE53-922A8A431F0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC37560-571E-403C-A77C-7F15B801E86A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{458BC130-9D90-47C7-8BCE-737B970934DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Test case 8</t>
+  </si>
+  <si>
+    <t>Test case 9</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +245,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0599683B-A5E9-44AE-92F5-D0FF41B6F4F8}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,14 +640,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -647,10 +656,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="23" t="s">
+      <c r="C3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -661,8 +670,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -699,44 +708,44 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="27">
         <v>1</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="28">
         <v>3</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="28">
         <v>3</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -745,10 +754,10 @@
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="23" t="s">
+      <c r="C13" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -759,8 +768,8 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -797,44 +806,44 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+      <c r="A18" s="27">
         <v>1</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="26">
-        <v>2</v>
-      </c>
-      <c r="E18" s="26">
-        <v>2</v>
-      </c>
-      <c r="F18" s="27" t="s">
+      <c r="D18" s="28">
+        <v>2</v>
+      </c>
+      <c r="E18" s="28">
+        <v>2</v>
+      </c>
+      <c r="F18" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -843,10 +852,10 @@
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="23" t="s">
+      <c r="C23" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -857,8 +866,8 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -895,44 +904,44 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="25">
+      <c r="A28" s="27">
         <v>1</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1">
         <v>8</v>
       </c>
-      <c r="D28" s="26">
-        <v>2</v>
-      </c>
-      <c r="E28" s="26">
-        <v>2</v>
-      </c>
-      <c r="F28" s="27" t="s">
+      <c r="D28" s="28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="28">
+        <v>2</v>
+      </c>
+      <c r="F28" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29"/>
     </row>
     <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -941,10 +950,10 @@
       <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="23" t="s">
+      <c r="C33" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -955,8 +964,8 @@
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -993,44 +1002,44 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="25">
+      <c r="A38" s="27">
         <v>1</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="1">
         <v>8</v>
       </c>
-      <c r="D38" s="26">
-        <v>4</v>
-      </c>
-      <c r="E38" s="26">
-        <v>4</v>
-      </c>
-      <c r="F38" s="27" t="s">
+      <c r="D38" s="28">
+        <v>4</v>
+      </c>
+      <c r="E38" s="28">
+        <v>4</v>
+      </c>
+      <c r="F38" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="10">
         <v>2</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="29"/>
     </row>
     <row r="41" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -1039,10 +1048,10 @@
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="23" t="s">
+      <c r="C43" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1053,8 +1062,8 @@
       <c r="B44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="26"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -1091,44 +1100,44 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="25">
+      <c r="A48" s="27">
         <v>1</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="1">
         <v>16</v>
       </c>
-      <c r="D48" s="26">
-        <v>2</v>
-      </c>
-      <c r="E48" s="26">
-        <v>2</v>
-      </c>
-      <c r="F48" s="27" t="s">
+      <c r="D48" s="28">
+        <v>2</v>
+      </c>
+      <c r="E48" s="28">
+        <v>2</v>
+      </c>
+      <c r="F48" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="26"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="12">
         <v>4</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="27"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
     </row>
     <row r="51" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
@@ -1137,10 +1146,10 @@
       <c r="B53" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" s="23" t="s">
+      <c r="C53" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1151,8 +1160,8 @@
       <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="26"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -1189,44 +1198,44 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="25">
+      <c r="A58" s="27">
         <v>1</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C58" s="1">
         <v>9</v>
       </c>
-      <c r="D58" s="26">
-        <v>2</v>
-      </c>
-      <c r="E58" s="26">
-        <v>2</v>
-      </c>
-      <c r="F58" s="27" t="s">
+      <c r="D58" s="28">
+        <v>2</v>
+      </c>
+      <c r="E58" s="28">
+        <v>2</v>
+      </c>
+      <c r="F58" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
-      <c r="B59" s="26"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="14">
         <v>3</v>
       </c>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="27"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="29"/>
     </row>
     <row r="61" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
@@ -1235,10 +1244,10 @@
       <c r="B63" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D63" s="23" t="s">
+      <c r="C63" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1249,8 +1258,8 @@
       <c r="B64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="26"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
@@ -1287,44 +1296,44 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="25">
+      <c r="A68" s="27">
         <v>1</v>
       </c>
-      <c r="B68" s="26" t="s">
+      <c r="B68" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C68" s="1">
         <v>20</v>
       </c>
-      <c r="D68" s="26">
+      <c r="D68" s="28">
         <v>3768</v>
       </c>
-      <c r="E68" s="26">
+      <c r="E68" s="28">
         <v>3768</v>
       </c>
-      <c r="F68" s="27" t="s">
+      <c r="F68" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
-      <c r="B69" s="26"/>
+      <c r="A69" s="27"/>
+      <c r="B69" s="28"/>
       <c r="C69" s="16">
         <v>3</v>
       </c>
-      <c r="D69" s="26"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="27"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="29"/>
     </row>
     <row r="71" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
@@ -1333,10 +1342,10 @@
       <c r="B73" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D73" s="23" t="s">
+      <c r="C73" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1347,8 +1356,8 @@
       <c r="B74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="24"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="26"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
@@ -1385,37 +1394,199 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="25">
+      <c r="A78" s="27">
         <v>1</v>
       </c>
-      <c r="B78" s="26" t="s">
+      <c r="B78" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C78" s="1">
         <v>5</v>
       </c>
-      <c r="D78" s="26">
+      <c r="D78" s="28">
         <v>157</v>
       </c>
-      <c r="E78" s="26">
+      <c r="E78" s="28">
         <v>157</v>
       </c>
-      <c r="F78" s="27" t="s">
+      <c r="F78" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="26"/>
+      <c r="A79" s="27"/>
+      <c r="B79" s="28"/>
       <c r="C79" s="18">
         <v>2</v>
       </c>
-      <c r="D79" s="26"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="27"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="29"/>
+    </row>
+    <row r="81" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A81" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" s="24"/>
+      <c r="D84" s="26"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="2">
+        <v>44534</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="27">
+        <v>1</v>
+      </c>
+      <c r="B88" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="1">
+        <v>10</v>
+      </c>
+      <c r="D88" s="28">
+        <v>1256</v>
+      </c>
+      <c r="E88" s="28">
+        <v>1256</v>
+      </c>
+      <c r="F88" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="27"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="20">
+        <v>4</v>
+      </c>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="72">
+    <mergeCell ref="A81:F81"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
     <mergeCell ref="A71:F71"/>
     <mergeCell ref="C73:C74"/>
     <mergeCell ref="D73:D74"/>
@@ -1424,62 +1595,6 @@
     <mergeCell ref="D78:D79"/>
     <mergeCell ref="E78:E79"/>
     <mergeCell ref="F78:F79"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>